<commit_message>
Down to joining in interventions.
</commit_message>
<xml_diff>
--- a/data/Energy Star_Energy Use by Calendar Month_US Properties.xlsx
+++ b/data/Energy Star_Energy Use by Calendar Month_US Properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{16AE6758-6275-439F-8AEB-6683597ABE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99259F03-FC30-4C23-BE9C-9AC42A57B616}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{16AE6758-6275-439F-8AEB-6683597ABE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B517F78-9910-4AA0-A472-C51F71EFBA19}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="923" firstSheet="17" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="923" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10 and 30 South Wacker" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="1099 New York Ave." sheetId="3" r:id="rId3"/>
     <sheet name="11 West 42nd Street" sheetId="4" r:id="rId4"/>
     <sheet name="1120 G Street, NW" sheetId="5" r:id="rId5"/>
-    <sheet name="11975 W Bluff Creek Drive " sheetId="6" r:id="rId6"/>
+    <sheet name="11975 W Bluff Creek Drive" sheetId="6" r:id="rId6"/>
     <sheet name="11985 W Bluff Creek Drive" sheetId="7" r:id="rId7"/>
     <sheet name="11995 W Bluff Creek Drive" sheetId="8" r:id="rId8"/>
     <sheet name="12005 W Bluff Creek Drive" sheetId="9" r:id="rId9"/>
@@ -36,7 +36,7 @@
     <sheet name="1730 Penn Ave." sheetId="21" r:id="rId21"/>
     <sheet name="1747 Penn Ave." sheetId="22" r:id="rId22"/>
     <sheet name="175 Varick" sheetId="23" r:id="rId23"/>
-    <sheet name="1775 Penn Ave. " sheetId="24" r:id="rId24"/>
+    <sheet name="1775 Penn Ave." sheetId="24" r:id="rId24"/>
     <sheet name="1919 Penn Ave." sheetId="25" r:id="rId25"/>
     <sheet name="2000 K" sheetId="26" r:id="rId26"/>
     <sheet name="2050 M Street" sheetId="27" r:id="rId27"/>
@@ -27668,7 +27668,7 @@
   </sheetPr>
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+    <sheetView topLeftCell="A60" workbookViewId="0">
       <selection activeCell="A68" sqref="A68:XFD83"/>
     </sheetView>
   </sheetViews>
@@ -31930,8 +31930,8 @@
   </sheetPr>
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32458,7 +32458,7 @@
   <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -59952,7 +59952,9 @@
   </sheetPr>
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>